<commit_message>
Added to fetch data from .xlsx by id
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -27,25 +27,34 @@
     <t>soyad</t>
   </si>
   <si>
-    <t>umut</t>
-  </si>
-  <si>
-    <t>ceylin</t>
-  </si>
-  <si>
-    <t>sevim</t>
-  </si>
-  <si>
-    <t>sadi</t>
-  </si>
-  <si>
-    <t>rabia</t>
-  </si>
-  <si>
     <t>sahin</t>
   </si>
   <si>
     <t>sayin</t>
+  </si>
+  <si>
+    <t>ali</t>
+  </si>
+  <si>
+    <t>ahmet</t>
+  </si>
+  <si>
+    <t>mehmet</t>
+  </si>
+  <si>
+    <t>seda</t>
+  </si>
+  <si>
+    <t>kerim</t>
+  </si>
+  <si>
+    <t>cicek</t>
+  </si>
+  <si>
+    <t>canan</t>
+  </si>
+  <si>
+    <t>aybar</t>
   </si>
 </sst>
 </file>
@@ -408,10 +417,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -419,10 +428,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -430,10 +439,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -441,10 +450,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -452,10 +461,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>